<commit_message>
Additional analysis individual datasets from Super-NaturalInstructions
</commit_message>
<xml_diff>
--- a/data/Super-NaturalInstructions/Task List.xlsx
+++ b/data/Super-NaturalInstructions/Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamweinberger/MIDS/compositional-reasoning-finetuning/data/Super-NaturalInstructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF332BDB-87B5-2E47-9E25-0712CC083E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C92E468-EEA1-CF4D-B83D-4FC0EED1A81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{A9AAB9C9-FD8F-B145-8CF8-FC02840DECF1}"/>
+    <workbookView xWindow="38400" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{A9AAB9C9-FD8F-B145-8CF8-FC02840DECF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9692" uniqueCount="3602">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9698" uniqueCount="3608">
   <si>
     <t>e</t>
   </si>
@@ -10845,6 +10845,24 @@
   </si>
   <si>
     <t>Check</t>
+  </si>
+  <si>
+    <t>Passages are about people moving from place to place</t>
+  </si>
+  <si>
+    <t>there is no way to model the reasoning step by step</t>
+  </si>
+  <si>
+    <t>pretty good</t>
+  </si>
+  <si>
+    <t>not possible to provide a structured explanation</t>
+  </si>
+  <si>
+    <t>kind of works for self-ask</t>
+  </si>
+  <si>
+    <t>has everything accept the evidences</t>
   </si>
 </sst>
 </file>
@@ -11204,16 +11222,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6483C-F321-0D4D-A0F0-EDCD3F74CCF4}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:G1616"/>
+  <dimension ref="A1:H1616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1350" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B1553" sqref="B1553"/>
+    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H294" sqref="H294"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="54.1640625" customWidth="1"/>
-    <col min="2" max="2" width="162" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="120.6640625" customWidth="1"/>
     <col min="3" max="3" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="6" width="5.5" customWidth="1"/>
   </cols>
@@ -11553,7 +11571,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>47</v>
       </c>
@@ -11573,7 +11591,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>49</v>
       </c>
@@ -11593,7 +11611,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>51</v>
       </c>
@@ -11613,7 +11631,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>53</v>
       </c>
@@ -11633,7 +11651,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>56</v>
       </c>
@@ -11653,7 +11671,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -11673,7 +11691,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>61</v>
       </c>
@@ -11693,7 +11711,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>64</v>
       </c>
@@ -11713,7 +11731,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>68</v>
       </c>
@@ -11733,7 +11751,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>70</v>
       </c>
@@ -11756,7 +11774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>72</v>
       </c>
@@ -11776,7 +11794,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>74</v>
       </c>
@@ -11796,7 +11814,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>77</v>
       </c>
@@ -11816,7 +11834,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>79</v>
       </c>
@@ -11838,8 +11856,11 @@
       <c r="G30">
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H30" t="s">
+        <v>3603</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>81</v>
       </c>
@@ -11859,7 +11880,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>84</v>
       </c>
@@ -12854,7 +12875,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
         <v>202</v>
       </c>
@@ -12874,7 +12895,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
         <v>205</v>
       </c>
@@ -12894,7 +12915,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
         <v>208</v>
       </c>
@@ -12914,7 +12935,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
         <v>210</v>
       </c>
@@ -12934,7 +12955,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
         <v>213</v>
       </c>
@@ -12956,8 +12977,11 @@
       <c r="G85">
         <v>2</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H85" t="s">
+        <v>3602</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
         <v>215</v>
       </c>
@@ -12980,7 +13004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
         <v>217</v>
       </c>
@@ -13000,7 +13024,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
         <v>219</v>
       </c>
@@ -13020,7 +13044,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
         <v>222</v>
       </c>
@@ -13040,7 +13064,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
         <v>224</v>
       </c>
@@ -13060,7 +13084,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
         <v>227</v>
       </c>
@@ -13080,7 +13104,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
         <v>231</v>
       </c>
@@ -13100,7 +13124,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
         <v>233</v>
       </c>
@@ -13120,7 +13144,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
         <v>236</v>
       </c>
@@ -13140,7 +13164,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
         <v>238</v>
       </c>
@@ -13160,7 +13184,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
         <v>240</v>
       </c>
@@ -14460,7 +14484,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>394</v>
       </c>
@@ -14480,7 +14504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>396</v>
       </c>
@@ -14500,7 +14524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>398</v>
       </c>
@@ -14520,7 +14544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>400</v>
       </c>
@@ -14540,7 +14564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>402</v>
       </c>
@@ -14560,7 +14584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>404</v>
       </c>
@@ -14580,7 +14604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>407</v>
       </c>
@@ -14600,7 +14624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>409</v>
       </c>
@@ -14620,7 +14644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>412</v>
       </c>
@@ -14640,7 +14664,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>414</v>
       </c>
@@ -14660,7 +14684,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>417</v>
       </c>
@@ -14680,7 +14704,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>419</v>
       </c>
@@ -14702,8 +14726,11 @@
       <c r="G172">
         <v>2</v>
       </c>
-    </row>
-    <row r="173" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H172" t="s">
+        <v>3604</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>421</v>
       </c>
@@ -14723,7 +14750,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="174" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>424</v>
       </c>
@@ -14743,7 +14770,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="175" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>427</v>
       </c>
@@ -14763,7 +14790,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="176" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>430</v>
       </c>
@@ -14783,7 +14810,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="177" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>433</v>
       </c>
@@ -14803,7 +14830,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="178" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>436</v>
       </c>
@@ -14825,8 +14852,11 @@
       <c r="G178">
         <v>2</v>
       </c>
-    </row>
-    <row r="179" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H178" t="s">
+        <v>3605</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>439</v>
       </c>
@@ -14846,7 +14876,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>441</v>
       </c>
@@ -14868,8 +14898,11 @@
       <c r="G180">
         <v>2</v>
       </c>
-    </row>
-    <row r="181" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H180" t="s">
+        <v>3606</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>443</v>
       </c>
@@ -14889,7 +14922,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>447</v>
       </c>
@@ -14909,7 +14942,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>449</v>
       </c>
@@ -14929,7 +14962,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>451</v>
       </c>
@@ -14949,7 +14982,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>454</v>
       </c>
@@ -14969,7 +15002,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>456</v>
       </c>
@@ -14989,7 +15022,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>458</v>
       </c>
@@ -15009,7 +15042,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>460</v>
       </c>
@@ -15029,7 +15062,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>462</v>
       </c>
@@ -15049,7 +15082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>464</v>
       </c>
@@ -15069,7 +15102,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>466</v>
       </c>
@@ -15089,7 +15122,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="192" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>468</v>
       </c>
@@ -15749,7 +15782,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>543</v>
       </c>
@@ -15769,7 +15802,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>545</v>
       </c>
@@ -15789,7 +15822,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>547</v>
       </c>
@@ -15809,7 +15842,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="228" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>549</v>
       </c>
@@ -15832,7 +15865,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>552</v>
       </c>
@@ -15852,7 +15885,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="230" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>554</v>
       </c>
@@ -15872,7 +15905,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>556</v>
       </c>
@@ -15895,7 +15928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>559</v>
       </c>
@@ -15918,7 +15951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>561</v>
       </c>
@@ -15938,7 +15971,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="234" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>563</v>
       </c>
@@ -15961,7 +15994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>565</v>
       </c>
@@ -15981,7 +16014,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="236" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>567</v>
       </c>
@@ -16001,7 +16034,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>569</v>
       </c>
@@ -16021,7 +16054,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="238" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>571</v>
       </c>
@@ -16041,7 +16074,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>573</v>
       </c>
@@ -16061,7 +16094,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="240" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>575</v>
       </c>
@@ -16082,6 +16115,9 @@
       </c>
       <c r="G240">
         <v>2</v>
+      </c>
+      <c r="H240" t="s">
+        <v>3607</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
finished adding chain of thought rationale to data_adaptor
</commit_message>
<xml_diff>
--- a/data/Super-NaturalInstructions/Task List.xlsx
+++ b/data/Super-NaturalInstructions/Task List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamweinberger/MIDS/compositional-reasoning-finetuning/data/Super-NaturalInstructions/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamweinberger/Library/CloudStorage/GoogleDrive-aandw1993@gmail.com/My Drive/MIDS/compositional-reasoning-finetuning/data/Super-NaturalInstructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C92E468-EEA1-CF4D-B83D-4FC0EED1A81B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9974B96B-791C-0345-9B32-A1134875609E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="760" windowWidth="34560" windowHeight="21580" xr2:uid="{A9AAB9C9-FD8F-B145-8CF8-FC02840DECF1}"/>
+    <workbookView xWindow="-19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{A9AAB9C9-FD8F-B145-8CF8-FC02840DECF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9698" uniqueCount="3608">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9706" uniqueCount="3616">
   <si>
     <t>e</t>
   </si>
@@ -10853,16 +10853,40 @@
     <t>there is no way to model the reasoning step by step</t>
   </si>
   <si>
-    <t>pretty good</t>
-  </si>
-  <si>
     <t>not possible to provide a structured explanation</t>
   </si>
   <si>
     <t>kind of works for self-ask</t>
   </si>
   <si>
-    <t>has everything accept the evidences</t>
+    <t>same as above</t>
+  </si>
+  <si>
+    <t>notes</t>
+  </si>
+  <si>
+    <t>fine_tuning</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>has everything except the evidences</t>
+  </si>
+  <si>
+    <t>It has context and evidence, but the evidence is pretty bad</t>
+  </si>
+  <si>
+    <t>hotpotqa, see above</t>
+  </si>
+  <si>
+    <t>not multi-hop</t>
+  </si>
+  <si>
+    <t>pretty good, 90k train examples, only issue is there is no evidences</t>
+  </si>
+  <si>
+    <t>This is supposed to be multi-hop, but when I read the questions they are not multi-up and often do not make sense. The readme does not correspond directly to the information in the dataset, 43k train</t>
   </si>
 </sst>
 </file>
@@ -11222,10 +11246,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4D6483C-F321-0D4D-A0F0-EDCD3F74CCF4}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H1616"/>
+  <dimension ref="A1:J1616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H294" sqref="H294"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B146" sqref="B146"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11236,7 +11260,7 @@
     <col min="4" max="6" width="5.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -11258,8 +11282,17 @@
       <c r="G1" t="s">
         <v>3601</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H1" t="s">
+        <v>3607</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3608</v>
+      </c>
+      <c r="J1" t="s">
+        <v>3609</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
@@ -11279,7 +11312,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>12</v>
       </c>
@@ -11299,7 +11332,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>18</v>
       </c>
@@ -11322,7 +11355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>21</v>
       </c>
@@ -11342,7 +11375,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>24</v>
       </c>
@@ -11365,7 +11398,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>26</v>
       </c>
@@ -11385,7 +11418,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -11405,7 +11438,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>31</v>
       </c>
@@ -11425,7 +11458,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
@@ -11445,7 +11478,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -11465,7 +11498,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
@@ -11488,7 +11521,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>39</v>
       </c>
@@ -11508,7 +11541,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>41</v>
       </c>
@@ -11528,7 +11561,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>43</v>
       </c>
@@ -11551,7 +11584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
@@ -14484,7 +14517,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A161" s="1" t="s">
         <v>394</v>
       </c>
@@ -14504,7 +14537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A162" s="1" t="s">
         <v>396</v>
       </c>
@@ -14524,7 +14557,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A163" s="1" t="s">
         <v>398</v>
       </c>
@@ -14544,7 +14577,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A164" s="1" t="s">
         <v>400</v>
       </c>
@@ -14564,7 +14597,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A165" s="1" t="s">
         <v>402</v>
       </c>
@@ -14584,7 +14617,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" s="1" t="s">
         <v>404</v>
       </c>
@@ -14604,7 +14637,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" s="1" t="s">
         <v>407</v>
       </c>
@@ -14624,7 +14657,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A168" s="1" t="s">
         <v>409</v>
       </c>
@@ -14644,7 +14677,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A169" s="1" t="s">
         <v>412</v>
       </c>
@@ -14664,7 +14697,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" s="1" t="s">
         <v>414</v>
       </c>
@@ -14684,7 +14717,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A171" s="1" t="s">
         <v>417</v>
       </c>
@@ -14704,7 +14737,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" s="1" t="s">
         <v>419</v>
       </c>
@@ -14727,10 +14760,16 @@
         <v>2</v>
       </c>
       <c r="H172" t="s">
-        <v>3604</v>
-      </c>
-    </row>
-    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+        <v>3614</v>
+      </c>
+      <c r="I172">
+        <v>1</v>
+      </c>
+      <c r="J172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A173" s="1" t="s">
         <v>421</v>
       </c>
@@ -14750,7 +14789,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A174" s="1" t="s">
         <v>424</v>
       </c>
@@ -14770,7 +14809,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A175" s="1" t="s">
         <v>427</v>
       </c>
@@ -14790,7 +14829,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A176" s="1" t="s">
         <v>430</v>
       </c>
@@ -14810,7 +14849,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A177" s="1" t="s">
         <v>433</v>
       </c>
@@ -14830,7 +14869,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" s="1" t="s">
         <v>436</v>
       </c>
@@ -14853,10 +14892,10 @@
         <v>2</v>
       </c>
       <c r="H178" t="s">
-        <v>3605</v>
-      </c>
-    </row>
-    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+        <v>3604</v>
+      </c>
+    </row>
+    <row r="179" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A179" s="1" t="s">
         <v>439</v>
       </c>
@@ -14876,7 +14915,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" s="1" t="s">
         <v>441</v>
       </c>
@@ -14899,10 +14938,16 @@
         <v>2</v>
       </c>
       <c r="H180" t="s">
-        <v>3606</v>
-      </c>
-    </row>
-    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+        <v>3605</v>
+      </c>
+      <c r="I180">
+        <v>1</v>
+      </c>
+      <c r="J180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A181" s="1" t="s">
         <v>443</v>
       </c>
@@ -14922,7 +14967,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A182" s="1" t="s">
         <v>447</v>
       </c>
@@ -14942,7 +14987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A183" s="1" t="s">
         <v>449</v>
       </c>
@@ -14962,7 +15007,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A184" s="1" t="s">
         <v>451</v>
       </c>
@@ -14982,7 +15027,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A185" s="1" t="s">
         <v>454</v>
       </c>
@@ -15002,7 +15047,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A186" s="1" t="s">
         <v>456</v>
       </c>
@@ -15022,7 +15067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A187" s="1" t="s">
         <v>458</v>
       </c>
@@ -15042,7 +15087,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A188" s="1" t="s">
         <v>460</v>
       </c>
@@ -15062,7 +15107,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A189" s="1" t="s">
         <v>462</v>
       </c>
@@ -15082,7 +15127,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A190" s="1" t="s">
         <v>464</v>
       </c>
@@ -15102,7 +15147,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A191" s="1" t="s">
         <v>466</v>
       </c>
@@ -15122,7 +15167,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
         <v>468</v>
       </c>
@@ -15782,7 +15827,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="225" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A225" s="1" t="s">
         <v>543</v>
       </c>
@@ -15802,7 +15847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="226" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A226" s="1" t="s">
         <v>545</v>
       </c>
@@ -15822,7 +15867,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="227" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A227" s="1" t="s">
         <v>547</v>
       </c>
@@ -15842,7 +15887,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="228" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228" s="1" t="s">
         <v>549</v>
       </c>
@@ -15865,7 +15910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="229" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A229" s="1" t="s">
         <v>552</v>
       </c>
@@ -15885,7 +15930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="230" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230" s="1" t="s">
         <v>554</v>
       </c>
@@ -15905,7 +15950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="231" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231" s="1" t="s">
         <v>556</v>
       </c>
@@ -15928,7 +15973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="232" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232" s="1" t="s">
         <v>559</v>
       </c>
@@ -15951,7 +15996,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="233" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233" s="1" t="s">
         <v>561</v>
       </c>
@@ -15971,7 +16016,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="234" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234" s="1" t="s">
         <v>563</v>
       </c>
@@ -15994,7 +16039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="235" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A235" s="1" t="s">
         <v>565</v>
       </c>
@@ -16014,7 +16059,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="236" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A236" s="1" t="s">
         <v>567</v>
       </c>
@@ -16034,7 +16079,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="237" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237" s="1" t="s">
         <v>569</v>
       </c>
@@ -16054,7 +16099,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="238" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A238" s="1" t="s">
         <v>571</v>
       </c>
@@ -16074,7 +16119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="239" spans="1:8" hidden="1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A239" s="1" t="s">
         <v>573</v>
       </c>
@@ -16094,7 +16139,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="240" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240" s="1" t="s">
         <v>575</v>
       </c>
@@ -16117,10 +16162,16 @@
         <v>2</v>
       </c>
       <c r="H240" t="s">
-        <v>3607</v>
-      </c>
-    </row>
-    <row r="241" spans="1:7" x14ac:dyDescent="0.2">
+        <v>3610</v>
+      </c>
+      <c r="I240">
+        <v>1</v>
+      </c>
+      <c r="J240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241" s="1" t="s">
         <v>577</v>
       </c>
@@ -16142,8 +16193,17 @@
       <c r="G241">
         <v>2</v>
       </c>
-    </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H241" t="s">
+        <v>3606</v>
+      </c>
+      <c r="I241">
+        <v>1</v>
+      </c>
+      <c r="J241">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242" s="1" t="s">
         <v>579</v>
       </c>
@@ -16166,7 +16226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="243" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A243" s="1" t="s">
         <v>581</v>
       </c>
@@ -16186,7 +16246,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="244" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A244" s="1" t="s">
         <v>583</v>
       </c>
@@ -16206,7 +16266,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="245" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A245" s="1" t="s">
         <v>585</v>
       </c>
@@ -16226,7 +16286,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="246" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A246" s="1" t="s">
         <v>587</v>
       </c>
@@ -16246,7 +16306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="247" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A247" s="1" t="s">
         <v>589</v>
       </c>
@@ -16266,7 +16326,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="248" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A248" s="1" t="s">
         <v>591</v>
       </c>
@@ -16286,7 +16346,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="249" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A249" s="1" t="s">
         <v>593</v>
       </c>
@@ -16306,7 +16366,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250" s="1" t="s">
         <v>596</v>
       </c>
@@ -16329,7 +16389,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251" s="1" t="s">
         <v>598</v>
       </c>
@@ -16349,7 +16409,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="252" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A252" s="1" t="s">
         <v>600</v>
       </c>
@@ -16369,7 +16429,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="253" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A253" s="1" t="s">
         <v>603</v>
       </c>
@@ -16389,7 +16449,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="254" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A254" s="1" t="s">
         <v>607</v>
       </c>
@@ -16409,7 +16469,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="255" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A255" s="1" t="s">
         <v>610</v>
       </c>
@@ -16429,7 +16489,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="256" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A256" s="1" t="s">
         <v>613</v>
       </c>
@@ -20304,7 +20364,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="449" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A449" s="1" t="s">
         <v>1064</v>
       </c>
@@ -20324,7 +20384,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="450" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A450" s="1" t="s">
         <v>1067</v>
       </c>
@@ -20344,7 +20404,7 @@
         <v>1069</v>
       </c>
     </row>
-    <row r="451" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A451" s="1" t="s">
         <v>1070</v>
       </c>
@@ -20364,7 +20424,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="452" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A452" s="1" t="s">
         <v>1073</v>
       </c>
@@ -20384,7 +20444,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="453" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A453" s="1" t="s">
         <v>1076</v>
       </c>
@@ -20404,7 +20464,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="454" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A454" s="1" t="s">
         <v>1079</v>
       </c>
@@ -20424,7 +20484,7 @@
         <v>1081</v>
       </c>
     </row>
-    <row r="455" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A455" s="1" t="s">
         <v>1082</v>
       </c>
@@ -20444,7 +20504,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="456" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A456" s="1" t="s">
         <v>1085</v>
       </c>
@@ -20464,7 +20524,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="457" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A457" s="1" t="s">
         <v>1088</v>
       </c>
@@ -20484,7 +20544,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="458" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A458" s="1" t="s">
         <v>1090</v>
       </c>
@@ -20504,7 +20564,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="459" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A459" s="1" t="s">
         <v>1092</v>
       </c>
@@ -20524,7 +20584,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="460" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A460" s="1" t="s">
         <v>1094</v>
       </c>
@@ -20544,7 +20604,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="461" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A461" s="1" t="s">
         <v>1096</v>
       </c>
@@ -20564,7 +20624,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="462" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A462" s="1" t="s">
         <v>1098</v>
       </c>
@@ -20586,8 +20646,17 @@
       <c r="G462">
         <v>2</v>
       </c>
-    </row>
-    <row r="463" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H462" t="s">
+        <v>3611</v>
+      </c>
+      <c r="I462">
+        <v>0</v>
+      </c>
+      <c r="J462">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="463" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A463" s="1" t="s">
         <v>1101</v>
       </c>
@@ -20607,7 +20676,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="464" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A464" s="1" t="s">
         <v>1103</v>
       </c>
@@ -36681,7 +36750,7 @@
         <v>2729</v>
       </c>
     </row>
-    <row r="1265" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1265" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1265" s="1" t="s">
         <v>2845</v>
       </c>
@@ -36701,7 +36770,7 @@
         <v>2450</v>
       </c>
     </row>
-    <row r="1266" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1266" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1266" s="1" t="s">
         <v>2847</v>
       </c>
@@ -36721,7 +36790,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="1267" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1267" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1267" s="1" t="s">
         <v>2849</v>
       </c>
@@ -36741,7 +36810,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="1268" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1268" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1268" s="1" t="s">
         <v>2851</v>
       </c>
@@ -36761,7 +36830,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="1269" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1269" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1269" s="1" t="s">
         <v>2853</v>
       </c>
@@ -36781,7 +36850,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1270" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1270" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1270" s="1" t="s">
         <v>2855</v>
       </c>
@@ -36801,7 +36870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1271" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1271" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1271" s="1" t="s">
         <v>2857</v>
       </c>
@@ -36821,7 +36890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1272" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1272" s="1" t="s">
         <v>2860</v>
       </c>
@@ -36841,7 +36910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1273" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1273" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1273" s="1" t="s">
         <v>2862</v>
       </c>
@@ -36861,7 +36930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1274" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1274" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1274" s="1" t="s">
         <v>2864</v>
       </c>
@@ -36881,7 +36950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1275" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1275" s="1" t="s">
         <v>2867</v>
       </c>
@@ -36901,7 +36970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1276" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1276" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1276" s="1" t="s">
         <v>2869</v>
       </c>
@@ -36921,7 +36990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1277" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1277" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1277" s="1" t="s">
         <v>2871</v>
       </c>
@@ -36941,7 +37010,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1278" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1278" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1278" s="1" t="s">
         <v>2873</v>
       </c>
@@ -36961,7 +37030,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1279" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1279" s="1" t="s">
         <v>2875</v>
       </c>
@@ -36983,8 +37052,17 @@
       <c r="G1279">
         <v>2</v>
       </c>
-    </row>
-    <row r="1280" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+      <c r="H1279" t="s">
+        <v>3612</v>
+      </c>
+      <c r="I1279">
+        <v>1</v>
+      </c>
+      <c r="J1279">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1280" s="1" t="s">
         <v>2877</v>
       </c>
@@ -37004,7 +37082,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1281" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1281" s="1" t="s">
         <v>2879</v>
       </c>
@@ -37026,8 +37104,11 @@
       <c r="G1281">
         <v>2</v>
       </c>
-    </row>
-    <row r="1282" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1281" t="s">
+        <v>3613</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1282" s="1" t="s">
         <v>2881</v>
       </c>
@@ -37049,8 +37130,17 @@
       <c r="G1282">
         <v>2</v>
       </c>
-    </row>
-    <row r="1283" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H1282" t="s">
+        <v>3615</v>
+      </c>
+      <c r="I1282">
+        <v>0</v>
+      </c>
+      <c r="J1282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1283" s="1" t="s">
         <v>2883</v>
       </c>
@@ -37070,7 +37160,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1284" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1284" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1284" s="1" t="s">
         <v>2885</v>
       </c>
@@ -37090,7 +37180,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1285" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1285" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1285" s="1" t="s">
         <v>2887</v>
       </c>
@@ -37110,7 +37200,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1286" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1286" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1286" s="1" t="s">
         <v>2889</v>
       </c>
@@ -37130,7 +37220,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1287" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1287" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1287" s="1" t="s">
         <v>2891</v>
       </c>
@@ -37150,7 +37240,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1288" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1288" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1288" s="1" t="s">
         <v>2893</v>
       </c>
@@ -37170,7 +37260,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1289" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1289" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1289" s="1" t="s">
         <v>2895</v>
       </c>
@@ -37190,7 +37280,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1290" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1290" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1290" s="1" t="s">
         <v>2897</v>
       </c>
@@ -37210,7 +37300,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1291" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1291" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1291" s="1" t="s">
         <v>2899</v>
       </c>
@@ -37230,7 +37320,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1292" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1292" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1292" s="1" t="s">
         <v>2901</v>
       </c>
@@ -37250,7 +37340,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1293" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1293" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1293" s="1" t="s">
         <v>2903</v>
       </c>
@@ -37270,7 +37360,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1294" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1294" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1294" s="1" t="s">
         <v>2905</v>
       </c>
@@ -37290,7 +37380,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1295" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1295" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1295" s="1" t="s">
         <v>2907</v>
       </c>
@@ -37310,7 +37400,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="1296" spans="1:7" hidden="1" x14ac:dyDescent="0.2">
+    <row r="1296" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
       <c r="A1296" s="1" t="s">
         <v>2909</v>
       </c>

</xml_diff>

<commit_message>
Added functionality for chain-of-thought answer before rationale
</commit_message>
<xml_diff>
--- a/data/Super-NaturalInstructions/Task List.xlsx
+++ b/data/Super-NaturalInstructions/Task List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/adamweinberger/Library/CloudStorage/GoogleDrive-aandw1993@gmail.com/My Drive/MIDS/compositional-reasoning-finetuning/data/Super-NaturalInstructions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9974B96B-791C-0345-9B32-A1134875609E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88088958-031B-7847-B47F-D9FD93B42598}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{A9AAB9C9-FD8F-B145-8CF8-FC02840DECF1}"/>
+    <workbookView xWindow="-38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{A9AAB9C9-FD8F-B145-8CF8-FC02840DECF1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -10856,9 +10856,6 @@
     <t>not possible to provide a structured explanation</t>
   </si>
   <si>
-    <t>kind of works for self-ask</t>
-  </si>
-  <si>
     <t>same as above</t>
   </si>
   <si>
@@ -10887,6 +10884,9 @@
   </si>
   <si>
     <t>This is supposed to be multi-hop, but when I read the questions they are not multi-up and often do not make sense. The readme does not correspond directly to the information in the dataset, 43k train</t>
+  </si>
+  <si>
+    <t>kind of works for self-ask but the one word answers aren't the only correct answer</t>
   </si>
 </sst>
 </file>
@@ -11248,8 +11248,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J1616"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11283,13 +11283,13 @@
         <v>3601</v>
       </c>
       <c r="H1" t="s">
+        <v>3606</v>
+      </c>
+      <c r="I1" t="s">
         <v>3607</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3608</v>
-      </c>
-      <c r="J1" t="s">
-        <v>3609</v>
       </c>
     </row>
     <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.2">
@@ -14760,7 +14760,7 @@
         <v>2</v>
       </c>
       <c r="H172" t="s">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="I172">
         <v>1</v>
@@ -14938,7 +14938,7 @@
         <v>2</v>
       </c>
       <c r="H180" t="s">
-        <v>3605</v>
+        <v>3615</v>
       </c>
       <c r="I180">
         <v>1</v>
@@ -16162,7 +16162,7 @@
         <v>2</v>
       </c>
       <c r="H240" t="s">
-        <v>3610</v>
+        <v>3609</v>
       </c>
       <c r="I240">
         <v>1</v>
@@ -16194,7 +16194,7 @@
         <v>2</v>
       </c>
       <c r="H241" t="s">
-        <v>3606</v>
+        <v>3605</v>
       </c>
       <c r="I241">
         <v>1</v>
@@ -20647,7 +20647,7 @@
         <v>2</v>
       </c>
       <c r="H462" t="s">
-        <v>3611</v>
+        <v>3610</v>
       </c>
       <c r="I462">
         <v>0</v>
@@ -37053,7 +37053,7 @@
         <v>2</v>
       </c>
       <c r="H1279" t="s">
-        <v>3612</v>
+        <v>3611</v>
       </c>
       <c r="I1279">
         <v>1</v>
@@ -37105,7 +37105,7 @@
         <v>2</v>
       </c>
       <c r="H1281" t="s">
-        <v>3613</v>
+        <v>3612</v>
       </c>
     </row>
     <row r="1282" spans="1:10" x14ac:dyDescent="0.2">
@@ -37131,7 +37131,7 @@
         <v>2</v>
       </c>
       <c r="H1282" t="s">
-        <v>3615</v>
+        <v>3614</v>
       </c>
       <c r="I1282">
         <v>0</v>

</xml_diff>